<commit_message>
fix: changement de calcul de l'évaluation du gain + corrections de la doc
</commit_message>
<xml_diff>
--- a/k8s-carbon-footprint-calculator.xlsx
+++ b/k8s-carbon-footprint-calculator.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\workspace\GreenIT\k8s-carbon-footprint\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{31C6915E-8692-4A47-AEB8-04AA45E56C44}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BD960542-DF72-49B9-BE64-15A674527AC9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13896" xr2:uid="{F5D5353E-3586-4AFE-B9F3-D539C270D077}"/>
   </bookViews>
@@ -101,9 +101,6 @@
     <t>Nb heures (période inactive) par an</t>
   </si>
   <si>
-    <t>Gain</t>
-  </si>
-  <si>
     <t>Consommation de CPU en moyenne</t>
   </si>
   <si>
@@ -296,6 +293,9 @@
   </si>
   <si>
     <t>GES (Conversion kWh =&gt; kgCO2eq) = 0,056 kgCO2eq/kWh</t>
+  </si>
+  <si>
+    <t>Evolution</t>
   </si>
 </sst>
 </file>
@@ -499,7 +499,7 @@
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="36">
+  <cellXfs count="34">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
@@ -516,31 +516,6 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="2" applyAlignment="1">
       <alignment horizontal="left" vertical="center" indent="10" readingOrder="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="11" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -560,32 +535,53 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="11" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="12" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="8" fillId="7" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -602,18 +598,6 @@
     </dxf>
     <dxf>
       <numFmt numFmtId="14" formatCode="0.00%"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
     </dxf>
     <dxf>
       <numFmt numFmtId="0" formatCode="General"/>
@@ -669,6 +653,18 @@
         </patternFill>
       </fill>
     </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
@@ -699,10 +695,10 @@
     <tableColumn id="19" xr3:uid="{57562154-D1A6-469C-A2A6-AAA01B1D74F2}" name="Nb heures (période inactive) par an">
       <calculatedColumnFormula>24*365-Tableau1[[#This Row],[Nb heures (période active) par an]]</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="10" xr3:uid="{CFCDDCD1-EF98-4164-AAD4-6D051056AEC8}" name="Energie (kWh) CPU sans kube-downscaler" totalsRowFunction="sum" dataDxfId="5">
+    <tableColumn id="10" xr3:uid="{CFCDDCD1-EF98-4164-AAD4-6D051056AEC8}" name="Energie (kWh) CPU sans kube-downscaler" totalsRowFunction="sum" dataDxfId="10">
       <calculatedColumnFormula array="1">(Tableau1[[#This Row],[CPUmoy (Période active)]]*Tableau1[[#This Row],[Nb heures (période active) par an]]+Tableau1[[#This Row],[CPUmoy (période inactive)]]*Tableau1[[#This Row],[Nb heures (période inactive) par an]])*Tableau2[kWh/CPU]*Tableau2[PUE]*Tableau1[[#This Row],[Nb de pods]]</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="21" xr3:uid="{D0904419-B936-43BE-BDF4-221DE5A72E53}" name="Energie (kWh) RAM sans kube-downscaler" totalsRowFunction="sum" dataDxfId="4">
+    <tableColumn id="21" xr3:uid="{D0904419-B936-43BE-BDF4-221DE5A72E53}" name="Energie (kWh) RAM sans kube-downscaler" totalsRowFunction="sum" dataDxfId="9">
       <calculatedColumnFormula array="1">(Tableau1[[#This Row],[RAMmoy (Période active)]]*Tableau1[[#This Row],[Nb heures (période active) par an]]+Tableau1[[#This Row],[RAMmoy (période inactive)]]*Tableau1[[#This Row],[Nb heures (période inactive) par an]])*Tableau2[kWh/GoRAM]*Tableau2[PUE]*Tableau1[[#This Row],[Nb de pods]]</calculatedColumnFormula>
     </tableColumn>
     <tableColumn id="22" xr3:uid="{47258D0C-0494-4D33-A55A-5D45CE9CD8BC}" name="Energie (kWh) totale sans kube-downscaler" totalsRowFunction="sum">
@@ -711,10 +707,10 @@
     <tableColumn id="23" xr3:uid="{A83A2756-33DE-458B-BA29-5C0C2A61B2BF}" name="kgCO2eq sans kube-downscaler" totalsRowFunction="sum">
       <calculatedColumnFormula array="1">Tableau1[[#This Row],[Energie (kWh) totale sans kube-downscaler]]*Tableau2[kgCO2/kWh]</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="11" xr3:uid="{FAFE4F05-7226-4132-A584-1C2377A24C37}" name="Energie (kWh) CPU avec kube-downscaler" totalsRowFunction="sum" dataDxfId="3">
+    <tableColumn id="11" xr3:uid="{FAFE4F05-7226-4132-A584-1C2377A24C37}" name="Energie (kWh) CPU avec kube-downscaler" totalsRowFunction="sum" dataDxfId="8">
       <calculatedColumnFormula array="1">Tableau1[[#This Row],[CPUmoy (Période active)]]*Tableau1[[#This Row],[Nb heures (période active) par an]]*Tableau2[kWh/CPU]*Tableau2[PUE]*Tableau1[[#This Row],[Nb de pods]]</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="13" xr3:uid="{A03F9329-AF52-4DA6-BCDF-578A92D93474}" name="Energie (kWh) RAM avec kube-downscaler" totalsRowFunction="sum" dataDxfId="2">
+    <tableColumn id="13" xr3:uid="{A03F9329-AF52-4DA6-BCDF-578A92D93474}" name="Energie (kWh) RAM avec kube-downscaler" totalsRowFunction="sum" dataDxfId="7">
       <calculatedColumnFormula array="1">Tableau1[[#This Row],[RAMmoy (Période active)]]*Tableau1[[#This Row],[Nb heures (période active) par an]]*Tableau2[kWh/GoRAM]*Tableau2[PUE]*Tableau1[[#This Row],[Nb de pods]]</calculatedColumnFormula>
     </tableColumn>
     <tableColumn id="15" xr3:uid="{5D8FBA35-CDBA-4C68-9E83-6835799B882B}" name="Energie (kWh) totale avec kube-downscaler" totalsRowFunction="sum">
@@ -723,9 +719,9 @@
     <tableColumn id="17" xr3:uid="{73C1DC75-42DF-478E-8AD5-15C822BC4D8D}" name="kgCO2eq avec kube-downscaler" totalsRowFunction="sum">
       <calculatedColumnFormula array="1">Tableau1[[#This Row],[Energie (kWh) totale avec kube-downscaler]]*Tableau2[kgCO2/kWh]</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="20" xr3:uid="{682833CB-1513-4B10-9167-85793868C041}" name="Gain" totalsRowFunction="custom" dataDxfId="1" totalsRowDxfId="0" dataCellStyle="Pourcentage">
-      <calculatedColumnFormula>Tableau1[[#This Row],[kgCO2eq avec kube-downscaler]]/Tableau1[[#This Row],[kgCO2eq sans kube-downscaler]]</calculatedColumnFormula>
-      <totalsRowFormula>Tableau1[[#Totals],[kgCO2eq avec kube-downscaler]]/Tableau1[[#Totals],[kgCO2eq sans kube-downscaler]]</totalsRowFormula>
+    <tableColumn id="20" xr3:uid="{682833CB-1513-4B10-9167-85793868C041}" name="Evolution" totalsRowFunction="custom" dataDxfId="1" totalsRowDxfId="0" dataCellStyle="Pourcentage">
+      <calculatedColumnFormula>(Tableau1[[#This Row],[kgCO2eq avec kube-downscaler]]-Tableau1[[#This Row],[kgCO2eq sans kube-downscaler]])/Tableau1[[#This Row],[kgCO2eq sans kube-downscaler]]</calculatedColumnFormula>
+      <totalsRowFormula>(Tableau1[[#Totals],[kgCO2eq avec kube-downscaler]]-Tableau1[[#Totals],[kgCO2eq sans kube-downscaler]])/Tableau1[[#Totals],[kgCO2eq sans kube-downscaler]]</totalsRowFormula>
     </tableColumn>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium4" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
@@ -733,10 +729,10 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{B2C602C2-FA01-4AEB-A7CE-4FFF16AEA4C4}" name="Tableau2" displayName="Tableau2" ref="A1:D2" totalsRowShown="0" headerRowDxfId="10" headerRowBorderDxfId="9" tableBorderDxfId="8" totalsRowBorderDxfId="7">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{B2C602C2-FA01-4AEB-A7CE-4FFF16AEA4C4}" name="Tableau2" displayName="Tableau2" ref="A1:D2" totalsRowShown="0" headerRowDxfId="6" headerRowBorderDxfId="5" tableBorderDxfId="4" totalsRowBorderDxfId="3">
   <autoFilter ref="A1:D2" xr:uid="{B2C602C2-FA01-4AEB-A7CE-4FFF16AEA4C4}"/>
   <tableColumns count="4">
-    <tableColumn id="1" xr3:uid="{75E3BE52-84B4-4CA9-A8BC-59D3569696C3}" name="kWh/CPU" dataDxfId="6">
+    <tableColumn id="1" xr3:uid="{75E3BE52-84B4-4CA9-A8BC-59D3569696C3}" name="kWh/CPU" dataDxfId="2">
       <calculatedColumnFormula>2.12/1000</calculatedColumnFormula>
     </tableColumn>
     <tableColumn id="2" xr3:uid="{68416F37-1DE6-4D24-8166-24F56C99900B}" name="kWh/GoRAM">
@@ -1070,8 +1066,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{97F58A1D-C50B-4ECA-A024-B8F8F3E1F1E5}">
   <dimension ref="A1:R9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F4" sqref="F4"/>
+    <sheetView tabSelected="1" zoomScale="93" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="Q12" sqref="Q12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" outlineLevelCol="1" x14ac:dyDescent="0.3"/>
@@ -1097,84 +1093,84 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A1" s="11" t="s">
+      <c r="A1" s="21" t="s">
+        <v>28</v>
+      </c>
+      <c r="B1" s="21"/>
+      <c r="C1" s="21"/>
+      <c r="D1" s="21"/>
+      <c r="E1" s="21"/>
+      <c r="F1" s="21"/>
+      <c r="G1" s="21"/>
+      <c r="H1" s="21"/>
+      <c r="I1" s="21"/>
+      <c r="J1" s="22" t="s">
         <v>29</v>
       </c>
-      <c r="B1" s="11"/>
-      <c r="C1" s="11"/>
-      <c r="D1" s="11"/>
-      <c r="E1" s="11"/>
-      <c r="F1" s="11"/>
-      <c r="G1" s="11"/>
-      <c r="H1" s="11"/>
-      <c r="I1" s="11"/>
-      <c r="J1" s="12" t="s">
+      <c r="K1" s="22"/>
+      <c r="L1" s="22"/>
+      <c r="M1" s="22"/>
+      <c r="N1" s="22"/>
+      <c r="O1" s="22"/>
+      <c r="P1" s="22"/>
+      <c r="Q1" s="22"/>
+    </row>
+    <row r="2" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A2" s="23" t="s">
         <v>30</v>
       </c>
-      <c r="K1" s="12"/>
-      <c r="L1" s="12"/>
-      <c r="M1" s="12"/>
-      <c r="N1" s="12"/>
-      <c r="O1" s="12"/>
-      <c r="P1" s="12"/>
-      <c r="Q1" s="12"/>
-    </row>
-    <row r="2" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A2" s="13" t="s">
-        <v>31</v>
-      </c>
-      <c r="B2" s="13"/>
-      <c r="C2" s="13"/>
-      <c r="D2" s="14" t="s">
+      <c r="B2" s="23"/>
+      <c r="C2" s="23"/>
+      <c r="D2" s="24" t="s">
+        <v>13</v>
+      </c>
+      <c r="E2" s="24"/>
+      <c r="F2" s="25" t="s">
         <v>14</v>
       </c>
-      <c r="E2" s="14"/>
-      <c r="F2" s="15" t="s">
+      <c r="G2" s="25"/>
+      <c r="H2" s="26" t="s">
         <v>15</v>
       </c>
-      <c r="G2" s="15"/>
-      <c r="H2" s="16" t="s">
+      <c r="I2" s="26"/>
+      <c r="J2" s="27" t="s">
         <v>16</v>
       </c>
-      <c r="I2" s="16"/>
-      <c r="J2" s="17" t="s">
+      <c r="K2" s="27"/>
+      <c r="L2" s="27"/>
+      <c r="M2" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="N2" s="20" t="s">
         <v>17</v>
       </c>
-      <c r="K2" s="17"/>
-      <c r="L2" s="17"/>
-      <c r="M2" s="3" t="s">
+      <c r="O2" s="20"/>
+      <c r="P2" s="20"/>
+      <c r="Q2" s="4" t="s">
         <v>19</v>
-      </c>
-      <c r="N2" s="10" t="s">
-        <v>18</v>
-      </c>
-      <c r="O2" s="10"/>
-      <c r="P2" s="10"/>
-      <c r="Q2" s="4" t="s">
-        <v>20</v>
       </c>
     </row>
     <row r="3" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
+        <v>21</v>
+      </c>
+      <c r="B3" t="s">
         <v>22</v>
       </c>
-      <c r="B3" t="s">
+      <c r="C3" t="s">
         <v>23</v>
       </c>
-      <c r="C3" t="s">
+      <c r="D3" t="s">
         <v>24</v>
       </c>
-      <c r="D3" t="s">
+      <c r="E3" t="s">
         <v>25</v>
       </c>
-      <c r="E3" t="s">
+      <c r="F3" t="s">
         <v>26</v>
       </c>
-      <c r="F3" t="s">
+      <c r="G3" t="s">
         <v>27</v>
-      </c>
-      <c r="G3" t="s">
-        <v>28</v>
       </c>
       <c r="H3" t="s">
         <v>11</v>
@@ -1207,15 +1203,15 @@
         <v>10</v>
       </c>
       <c r="R3" t="s">
-        <v>13</v>
+        <v>77</v>
       </c>
     </row>
     <row r="4" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B4" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C4">
         <v>2</v>
@@ -1273,16 +1269,16 @@
         <v>0.86381568000000009</v>
       </c>
       <c r="R4" s="2">
-        <f>Tableau1[[#This Row],[kgCO2eq avec kube-downscaler]]/Tableau1[[#This Row],[kgCO2eq sans kube-downscaler]]</f>
-        <v>0.47391939123125248</v>
+        <f>(Tableau1[[#This Row],[kgCO2eq avec kube-downscaler]]-Tableau1[[#This Row],[kgCO2eq sans kube-downscaler]])/Tableau1[[#This Row],[kgCO2eq sans kube-downscaler]]</f>
+        <v>-0.52608060876874752</v>
       </c>
     </row>
     <row r="5" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B5" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C5">
         <v>2</v>
@@ -1307,11 +1303,11 @@
         <f>24*365-Tableau1[[#This Row],[Nb heures (période active) par an]]</f>
         <v>5640</v>
       </c>
-      <c r="J5" s="18" cm="1">
+      <c r="J5" cm="1">
         <f t="array" ref="J5">(Tableau1[[#This Row],[CPUmoy (Période active)]]*Tableau1[[#This Row],[Nb heures (période active) par an]]+Tableau1[[#This Row],[CPUmoy (période inactive)]]*Tableau1[[#This Row],[Nb heures (période inactive) par an]])*Tableau2[kWh/CPU]*Tableau2[PUE]*Tableau1[[#This Row],[Nb de pods]]</f>
         <v>17.095679999999998</v>
       </c>
-      <c r="K5" s="18" cm="1">
+      <c r="K5" cm="1">
         <f t="array" ref="K5">(Tableau1[[#This Row],[RAMmoy (Période active)]]*Tableau1[[#This Row],[Nb heures (période active) par an]]+Tableau1[[#This Row],[RAMmoy (période inactive)]]*Tableau1[[#This Row],[Nb heures (période inactive) par an]])*Tableau2[kWh/GoRAM]*Tableau2[PUE]*Tableau1[[#This Row],[Nb de pods]]</f>
         <v>15.452640000000002</v>
       </c>
@@ -1323,11 +1319,11 @@
         <f t="array" ref="M5">Tableau1[[#This Row],[Energie (kWh) totale sans kube-downscaler]]*Tableau2[kgCO2/kWh]</f>
         <v>1.8227059200000002</v>
       </c>
-      <c r="N5" s="18" cm="1">
+      <c r="N5" cm="1">
         <f t="array" ref="N5">Tableau1[[#This Row],[CPUmoy (Période active)]]*Tableau1[[#This Row],[Nb heures (période active) par an]]*Tableau2[kWh/CPU]*Tableau2[PUE]*Tableau1[[#This Row],[Nb de pods]]</f>
         <v>9.9215999999999998</v>
       </c>
-      <c r="O5" s="18" cm="1">
+      <c r="O5" cm="1">
         <f t="array" ref="O5">Tableau1[[#This Row],[RAMmoy (Période active)]]*Tableau1[[#This Row],[Nb heures (période active) par an]]*Tableau2[kWh/GoRAM]*Tableau2[PUE]*Tableau1[[#This Row],[Nb de pods]]</f>
         <v>5.503680000000001</v>
       </c>
@@ -1340,16 +1336,16 @@
         <v>0.86381568000000009</v>
       </c>
       <c r="R5" s="2">
-        <f>Tableau1[[#This Row],[kgCO2eq avec kube-downscaler]]/Tableau1[[#This Row],[kgCO2eq sans kube-downscaler]]</f>
-        <v>0.47391939123125248</v>
+        <f>(Tableau1[[#This Row],[kgCO2eq avec kube-downscaler]]-Tableau1[[#This Row],[kgCO2eq sans kube-downscaler]])/Tableau1[[#This Row],[kgCO2eq sans kube-downscaler]]</f>
+        <v>-0.52608060876874752</v>
       </c>
     </row>
     <row r="6" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B6" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C6">
         <v>3</v>
@@ -1374,11 +1370,11 @@
         <f>24*365-Tableau1[[#This Row],[Nb heures (période active) par an]]</f>
         <v>5640</v>
       </c>
-      <c r="J6" s="18" cm="1">
+      <c r="J6" cm="1">
         <f t="array" ref="J6">(Tableau1[[#This Row],[CPUmoy (Période active)]]*Tableau1[[#This Row],[Nb heures (période active) par an]]+Tableau1[[#This Row],[CPUmoy (période inactive)]]*Tableau1[[#This Row],[Nb heures (période inactive) par an]])*Tableau2[kWh/CPU]*Tableau2[PUE]*Tableau1[[#This Row],[Nb de pods]]</f>
         <v>36.977039999999995</v>
       </c>
-      <c r="K6" s="18" cm="1">
+      <c r="K6" cm="1">
         <f t="array" ref="K6">(Tableau1[[#This Row],[RAMmoy (Période active)]]*Tableau1[[#This Row],[Nb heures (période active) par an]]+Tableau1[[#This Row],[RAMmoy (période inactive)]]*Tableau1[[#This Row],[Nb heures (période inactive) par an]])*Tableau2[kWh/GoRAM]*Tableau2[PUE]*Tableau1[[#This Row],[Nb de pods]]</f>
         <v>23.178960000000004</v>
       </c>
@@ -1390,11 +1386,11 @@
         <f t="array" ref="M6">Tableau1[[#This Row],[Energie (kWh) totale sans kube-downscaler]]*Tableau2[kgCO2/kWh]</f>
         <v>3.3687360000000002</v>
       </c>
-      <c r="N6" s="18" cm="1">
+      <c r="N6" cm="1">
         <f t="array" ref="N6">Tableau1[[#This Row],[CPUmoy (Période active)]]*Tableau1[[#This Row],[Nb heures (période active) par an]]*Tableau2[kWh/CPU]*Tableau2[PUE]*Tableau1[[#This Row],[Nb de pods]]</f>
         <v>20.835359999999998</v>
       </c>
-      <c r="O6" s="18" cm="1">
+      <c r="O6" cm="1">
         <f t="array" ref="O6">Tableau1[[#This Row],[RAMmoy (Période active)]]*Tableau1[[#This Row],[Nb heures (période active) par an]]*Tableau2[kWh/GoRAM]*Tableau2[PUE]*Tableau1[[#This Row],[Nb de pods]]</f>
         <v>8.2555200000000006</v>
       </c>
@@ -1407,16 +1403,16 @@
         <v>1.6290892799999999</v>
       </c>
       <c r="R6" s="2">
-        <f>Tableau1[[#This Row],[kgCO2eq avec kube-downscaler]]/Tableau1[[#This Row],[kgCO2eq sans kube-downscaler]]</f>
-        <v>0.48359066427289044</v>
+        <f>(Tableau1[[#This Row],[kgCO2eq avec kube-downscaler]]-Tableau1[[#This Row],[kgCO2eq sans kube-downscaler]])/Tableau1[[#This Row],[kgCO2eq sans kube-downscaler]]</f>
+        <v>-0.51640933572710956</v>
       </c>
     </row>
     <row r="7" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B7" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C7">
         <v>5</v>
@@ -1441,11 +1437,11 @@
         <f>24*365-Tableau1[[#This Row],[Nb heures (période active) par an]]</f>
         <v>5640</v>
       </c>
-      <c r="J7" s="18" cm="1">
+      <c r="J7" cm="1">
         <f t="array" ref="J7">(Tableau1[[#This Row],[CPUmoy (Période active)]]*Tableau1[[#This Row],[Nb heures (période active) par an]]+Tableau1[[#This Row],[CPUmoy (période inactive)]]*Tableau1[[#This Row],[Nb heures (période inactive) par an]])*Tableau2[kWh/CPU]*Tableau2[PUE]*Tableau1[[#This Row],[Nb de pods]]</f>
         <v>76.510800000000003</v>
       </c>
-      <c r="K7" s="18" cm="1">
+      <c r="K7" cm="1">
         <f t="array" ref="K7">(Tableau1[[#This Row],[RAMmoy (Période active)]]*Tableau1[[#This Row],[Nb heures (période active) par an]]+Tableau1[[#This Row],[RAMmoy (période inactive)]]*Tableau1[[#This Row],[Nb heures (période inactive) par an]])*Tableau2[kWh/GoRAM]*Tableau2[PUE]*Tableau1[[#This Row],[Nb de pods]]</f>
         <v>46.357920000000007</v>
       </c>
@@ -1457,11 +1453,11 @@
         <f t="array" ref="M7">Tableau1[[#This Row],[Energie (kWh) totale sans kube-downscaler]]*Tableau2[kgCO2/kWh]</f>
         <v>6.8806483200000006</v>
       </c>
-      <c r="N7" s="18" cm="1">
+      <c r="N7" cm="1">
         <f t="array" ref="N7">Tableau1[[#This Row],[CPUmoy (Période active)]]*Tableau1[[#This Row],[Nb heures (période active) par an]]*Tableau2[kWh/CPU]*Tableau2[PUE]*Tableau1[[#This Row],[Nb de pods]]</f>
         <v>49.607999999999997</v>
       </c>
-      <c r="O7" s="18" cm="1">
+      <c r="O7" cm="1">
         <f t="array" ref="O7">Tableau1[[#This Row],[RAMmoy (Période active)]]*Tableau1[[#This Row],[Nb heures (période active) par an]]*Tableau2[kWh/GoRAM]*Tableau2[PUE]*Tableau1[[#This Row],[Nb de pods]]</f>
         <v>16.511040000000001</v>
       </c>
@@ -1474,16 +1470,16 @@
         <v>3.7026662400000001</v>
       </c>
       <c r="R7" s="2">
-        <f>Tableau1[[#This Row],[kgCO2eq avec kube-downscaler]]/Tableau1[[#This Row],[kgCO2eq sans kube-downscaler]]</f>
-        <v>0.53812752342500192</v>
+        <f>(Tableau1[[#This Row],[kgCO2eq avec kube-downscaler]]-Tableau1[[#This Row],[kgCO2eq sans kube-downscaler]])/Tableau1[[#This Row],[kgCO2eq sans kube-downscaler]]</f>
+        <v>-0.46187247657499814</v>
       </c>
     </row>
     <row r="8" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B8" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C8">
         <v>5</v>
@@ -1508,11 +1504,11 @@
         <f>24*365-Tableau1[[#This Row],[Nb heures (période active) par an]]</f>
         <v>5640</v>
       </c>
-      <c r="J8" s="18" cm="1">
+      <c r="J8" cm="1">
         <f t="array" ref="J8">(Tableau1[[#This Row],[CPUmoy (Période active)]]*Tableau1[[#This Row],[Nb heures (période active) par an]]+Tableau1[[#This Row],[CPUmoy (période inactive)]]*Tableau1[[#This Row],[Nb heures (période inactive) par an]])*Tableau2[kWh/CPU]*Tableau2[PUE]*Tableau1[[#This Row],[Nb de pods]]</f>
         <v>76.510800000000003</v>
       </c>
-      <c r="K8" s="18" cm="1">
+      <c r="K8" cm="1">
         <f t="array" ref="K8">(Tableau1[[#This Row],[RAMmoy (Période active)]]*Tableau1[[#This Row],[Nb heures (période active) par an]]+Tableau1[[#This Row],[RAMmoy (période inactive)]]*Tableau1[[#This Row],[Nb heures (période inactive) par an]])*Tableau2[kWh/GoRAM]*Tableau2[PUE]*Tableau1[[#This Row],[Nb de pods]]</f>
         <v>46.357920000000007</v>
       </c>
@@ -1524,11 +1520,11 @@
         <f t="array" ref="M8">Tableau1[[#This Row],[Energie (kWh) totale sans kube-downscaler]]*Tableau2[kgCO2/kWh]</f>
         <v>6.8806483200000006</v>
       </c>
-      <c r="N8" s="18" cm="1">
+      <c r="N8" cm="1">
         <f t="array" ref="N8">Tableau1[[#This Row],[CPUmoy (Période active)]]*Tableau1[[#This Row],[Nb heures (période active) par an]]*Tableau2[kWh/CPU]*Tableau2[PUE]*Tableau1[[#This Row],[Nb de pods]]</f>
         <v>49.607999999999997</v>
       </c>
-      <c r="O8" s="18" cm="1">
+      <c r="O8" cm="1">
         <f t="array" ref="O8">Tableau1[[#This Row],[RAMmoy (Période active)]]*Tableau1[[#This Row],[Nb heures (période active) par an]]*Tableau2[kWh/GoRAM]*Tableau2[PUE]*Tableau1[[#This Row],[Nb de pods]]</f>
         <v>16.511040000000001</v>
       </c>
@@ -1541,13 +1537,13 @@
         <v>3.7026662400000001</v>
       </c>
       <c r="R8" s="2">
-        <f>Tableau1[[#This Row],[kgCO2eq avec kube-downscaler]]/Tableau1[[#This Row],[kgCO2eq sans kube-downscaler]]</f>
-        <v>0.53812752342500192</v>
+        <f>(Tableau1[[#This Row],[kgCO2eq avec kube-downscaler]]-Tableau1[[#This Row],[kgCO2eq sans kube-downscaler]])/Tableau1[[#This Row],[kgCO2eq sans kube-downscaler]]</f>
+        <v>-0.46187247657499814</v>
       </c>
     </row>
     <row r="9" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="J9">
         <f>SUBTOTAL(109,Tableau1[Energie (kWh) CPU sans kube-downscaler])</f>
@@ -1581,9 +1577,9 @@
         <f>SUBTOTAL(109,Tableau1[kgCO2eq avec kube-downscaler])</f>
         <v>10.762053120000001</v>
       </c>
-      <c r="R9" s="19">
-        <f>Tableau1[[#Totals],[kgCO2eq avec kube-downscaler]]/Tableau1[[#Totals],[kgCO2eq sans kube-downscaler]]</f>
-        <v>0.51801794808098367</v>
+      <c r="R9" s="10">
+        <f>(Tableau1[[#Totals],[kgCO2eq avec kube-downscaler]]-Tableau1[[#Totals],[kgCO2eq sans kube-downscaler]])/Tableau1[[#Totals],[kgCO2eq sans kube-downscaler]]</f>
+        <v>-0.48198205191901633</v>
       </c>
     </row>
   </sheetData>
@@ -1629,7 +1625,7 @@
         <v>2</v>
       </c>
       <c r="D1" s="5" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.3">
@@ -1682,208 +1678,208 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A1" s="30" t="s">
+      <c r="A1" s="28" t="s">
+        <v>38</v>
+      </c>
+      <c r="B1" s="28"/>
+      <c r="C1" s="28"/>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A2" s="13" t="s">
+        <v>40</v>
+      </c>
+      <c r="B2" s="13" t="s">
+        <v>41</v>
+      </c>
+      <c r="C2" s="13" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A3" s="14" t="s">
         <v>39</v>
       </c>
-      <c r="B1" s="30"/>
-      <c r="C1" s="30"/>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A2" s="22" t="s">
-        <v>41</v>
-      </c>
-      <c r="B2" s="22" t="s">
+      <c r="B3" s="15" t="s">
         <v>42</v>
       </c>
-      <c r="C2" s="22" t="s">
+      <c r="C3" s="16" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="3" spans="1:3" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A3" s="23" t="s">
-        <v>40</v>
-      </c>
-      <c r="B3" s="24" t="s">
-        <v>43</v>
-      </c>
-      <c r="C3" s="25" t="s">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A4" s="14" t="s">
         <v>45</v>
       </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A4" s="23" t="s">
+      <c r="B4" s="15" t="s">
+        <v>42</v>
+      </c>
+      <c r="C4" s="14"/>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A5" s="14" t="s">
+        <v>76</v>
+      </c>
+      <c r="B5" s="15" t="s">
         <v>46</v>
       </c>
-      <c r="B4" s="24" t="s">
-        <v>43</v>
-      </c>
-      <c r="C4" s="23"/>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A5" s="23" t="s">
-        <v>77</v>
-      </c>
-      <c r="B5" s="24" t="s">
+      <c r="C5" s="14" t="s">
         <v>47</v>
       </c>
-      <c r="C5" s="23" t="s">
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A6" s="14" t="s">
         <v>48</v>
       </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A6" s="23" t="s">
+      <c r="B6" s="14"/>
+      <c r="C6" s="14" t="s">
         <v>49</v>
       </c>
-      <c r="B6" s="23"/>
-      <c r="C6" s="23" t="s">
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A8" s="29" t="s">
+        <v>53</v>
+      </c>
+      <c r="B8" s="29"/>
+      <c r="C8" s="29"/>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A9" s="18" t="s">
+        <v>54</v>
+      </c>
+      <c r="B9" s="19" t="s">
+        <v>55</v>
+      </c>
+      <c r="C9" s="19" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A10" s="16" t="s">
+        <v>21</v>
+      </c>
+      <c r="B10" s="12" t="s">
+        <v>57</v>
+      </c>
+      <c r="C10" s="12" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A11" s="16" t="s">
+        <v>22</v>
+      </c>
+      <c r="B11" s="12" t="s">
+        <v>59</v>
+      </c>
+      <c r="C11" s="12" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A12" s="16" t="s">
+        <v>23</v>
+      </c>
+      <c r="B12" s="12" t="s">
+        <v>60</v>
+      </c>
+      <c r="C12" s="12" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A13" s="16" t="s">
+        <v>24</v>
+      </c>
+      <c r="B13" s="12" t="s">
+        <v>63</v>
+      </c>
+      <c r="C13" s="12" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A14" s="12" t="s">
+        <v>65</v>
+      </c>
+      <c r="B14" s="12" t="s">
+        <v>66</v>
+      </c>
+      <c r="C14" s="12" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A15" s="16" t="s">
+        <v>26</v>
+      </c>
+      <c r="B15" s="12" t="s">
+        <v>68</v>
+      </c>
+      <c r="C15" s="12" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A16" s="12" t="s">
+        <v>70</v>
+      </c>
+      <c r="B16" s="12" t="s">
+        <v>69</v>
+      </c>
+      <c r="C16" s="12" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A17" s="11"/>
+      <c r="B17" s="11"/>
+      <c r="C17" s="11"/>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A18" s="31" t="s">
         <v>50</v>
       </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A8" s="31" t="s">
-        <v>54</v>
-      </c>
-      <c r="B8" s="31"/>
-      <c r="C8" s="31"/>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A9" s="28" t="s">
-        <v>55</v>
-      </c>
-      <c r="B9" s="29" t="s">
-        <v>56</v>
-      </c>
-      <c r="C9" s="29" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A10" s="27" t="s">
-        <v>22</v>
-      </c>
-      <c r="B10" s="21" t="s">
-        <v>58</v>
-      </c>
-      <c r="C10" s="21" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A11" s="27" t="s">
-        <v>23</v>
-      </c>
-      <c r="B11" s="21" t="s">
-        <v>60</v>
-      </c>
-      <c r="C11" s="21" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A12" s="27" t="s">
-        <v>24</v>
-      </c>
-      <c r="B12" s="21" t="s">
-        <v>61</v>
-      </c>
-      <c r="C12" s="21" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A13" s="27" t="s">
-        <v>25</v>
-      </c>
-      <c r="B13" s="21" t="s">
-        <v>64</v>
-      </c>
-      <c r="C13" s="21" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A14" s="21" t="s">
-        <v>66</v>
-      </c>
-      <c r="B14" s="21" t="s">
-        <v>67</v>
-      </c>
-      <c r="C14" s="21" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A15" s="27" t="s">
-        <v>27</v>
-      </c>
-      <c r="B15" s="21" t="s">
-        <v>69</v>
-      </c>
-      <c r="C15" s="21" t="s">
+      <c r="B18" s="32"/>
+      <c r="C18" s="32"/>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A19" s="30" t="s">
+        <v>51</v>
+      </c>
+      <c r="B19" s="30"/>
+      <c r="C19" s="30"/>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A20" s="30" t="s">
+        <v>52</v>
+      </c>
+      <c r="B20" s="30"/>
+      <c r="C20" s="30"/>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A21" s="33" t="s">
         <v>73</v>
       </c>
-    </row>
-    <row r="16" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A16" s="21" t="s">
-        <v>71</v>
-      </c>
-      <c r="B16" s="21" t="s">
-        <v>70</v>
-      </c>
-      <c r="C16" s="21" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A17" s="20"/>
-      <c r="B17" s="20"/>
-      <c r="C17" s="20"/>
-    </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A18" s="32" t="s">
-        <v>51</v>
-      </c>
-      <c r="B18" s="33"/>
-      <c r="C18" s="33"/>
-    </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A19" s="34" t="s">
-        <v>52</v>
-      </c>
-      <c r="B19" s="34"/>
-      <c r="C19" s="34"/>
-    </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A20" s="34" t="s">
-        <v>53</v>
-      </c>
-      <c r="B20" s="34"/>
-      <c r="C20" s="34"/>
-    </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A21" s="35" t="s">
+      <c r="B21" s="33"/>
+      <c r="C21" s="33"/>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A22" s="33" t="s">
         <v>74</v>
       </c>
-      <c r="B21" s="35"/>
-      <c r="C21" s="35"/>
-    </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A22" s="35" t="s">
+      <c r="B22" s="33"/>
+      <c r="C22" s="33"/>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A23" s="30" t="s">
         <v>75</v>
       </c>
-      <c r="B22" s="35"/>
-      <c r="C22" s="35"/>
-    </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A23" s="34" t="s">
-        <v>76</v>
-      </c>
-      <c r="B23" s="34"/>
-      <c r="C23" s="34"/>
+      <c r="B23" s="30"/>
+      <c r="C23" s="30"/>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="B24" s="26"/>
-      <c r="C24" s="26"/>
+      <c r="B24" s="17"/>
+      <c r="C24" s="17"/>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A26" s="9"/>

</xml_diff>

<commit_message>
fix: changement de calcul de l'évaluation du gain + corrections de la doc (#2)
Co-authored-by: PREISNER Julien <julien.preisner@soprasteria.com>
</commit_message>
<xml_diff>
--- a/k8s-carbon-footprint-calculator.xlsx
+++ b/k8s-carbon-footprint-calculator.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\workspace\GreenIT\k8s-carbon-footprint\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{31C6915E-8692-4A47-AEB8-04AA45E56C44}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BD960542-DF72-49B9-BE64-15A674527AC9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13896" xr2:uid="{F5D5353E-3586-4AFE-B9F3-D539C270D077}"/>
   </bookViews>
@@ -101,9 +101,6 @@
     <t>Nb heures (période inactive) par an</t>
   </si>
   <si>
-    <t>Gain</t>
-  </si>
-  <si>
     <t>Consommation de CPU en moyenne</t>
   </si>
   <si>
@@ -296,6 +293,9 @@
   </si>
   <si>
     <t>GES (Conversion kWh =&gt; kgCO2eq) = 0,056 kgCO2eq/kWh</t>
+  </si>
+  <si>
+    <t>Evolution</t>
   </si>
 </sst>
 </file>
@@ -499,7 +499,7 @@
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="36">
+  <cellXfs count="34">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
@@ -516,31 +516,6 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="2" applyAlignment="1">
       <alignment horizontal="left" vertical="center" indent="10" readingOrder="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="11" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -560,32 +535,53 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="11" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="12" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="8" fillId="7" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -602,18 +598,6 @@
     </dxf>
     <dxf>
       <numFmt numFmtId="14" formatCode="0.00%"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
     </dxf>
     <dxf>
       <numFmt numFmtId="0" formatCode="General"/>
@@ -669,6 +653,18 @@
         </patternFill>
       </fill>
     </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
@@ -699,10 +695,10 @@
     <tableColumn id="19" xr3:uid="{57562154-D1A6-469C-A2A6-AAA01B1D74F2}" name="Nb heures (période inactive) par an">
       <calculatedColumnFormula>24*365-Tableau1[[#This Row],[Nb heures (période active) par an]]</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="10" xr3:uid="{CFCDDCD1-EF98-4164-AAD4-6D051056AEC8}" name="Energie (kWh) CPU sans kube-downscaler" totalsRowFunction="sum" dataDxfId="5">
+    <tableColumn id="10" xr3:uid="{CFCDDCD1-EF98-4164-AAD4-6D051056AEC8}" name="Energie (kWh) CPU sans kube-downscaler" totalsRowFunction="sum" dataDxfId="10">
       <calculatedColumnFormula array="1">(Tableau1[[#This Row],[CPUmoy (Période active)]]*Tableau1[[#This Row],[Nb heures (période active) par an]]+Tableau1[[#This Row],[CPUmoy (période inactive)]]*Tableau1[[#This Row],[Nb heures (période inactive) par an]])*Tableau2[kWh/CPU]*Tableau2[PUE]*Tableau1[[#This Row],[Nb de pods]]</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="21" xr3:uid="{D0904419-B936-43BE-BDF4-221DE5A72E53}" name="Energie (kWh) RAM sans kube-downscaler" totalsRowFunction="sum" dataDxfId="4">
+    <tableColumn id="21" xr3:uid="{D0904419-B936-43BE-BDF4-221DE5A72E53}" name="Energie (kWh) RAM sans kube-downscaler" totalsRowFunction="sum" dataDxfId="9">
       <calculatedColumnFormula array="1">(Tableau1[[#This Row],[RAMmoy (Période active)]]*Tableau1[[#This Row],[Nb heures (période active) par an]]+Tableau1[[#This Row],[RAMmoy (période inactive)]]*Tableau1[[#This Row],[Nb heures (période inactive) par an]])*Tableau2[kWh/GoRAM]*Tableau2[PUE]*Tableau1[[#This Row],[Nb de pods]]</calculatedColumnFormula>
     </tableColumn>
     <tableColumn id="22" xr3:uid="{47258D0C-0494-4D33-A55A-5D45CE9CD8BC}" name="Energie (kWh) totale sans kube-downscaler" totalsRowFunction="sum">
@@ -711,10 +707,10 @@
     <tableColumn id="23" xr3:uid="{A83A2756-33DE-458B-BA29-5C0C2A61B2BF}" name="kgCO2eq sans kube-downscaler" totalsRowFunction="sum">
       <calculatedColumnFormula array="1">Tableau1[[#This Row],[Energie (kWh) totale sans kube-downscaler]]*Tableau2[kgCO2/kWh]</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="11" xr3:uid="{FAFE4F05-7226-4132-A584-1C2377A24C37}" name="Energie (kWh) CPU avec kube-downscaler" totalsRowFunction="sum" dataDxfId="3">
+    <tableColumn id="11" xr3:uid="{FAFE4F05-7226-4132-A584-1C2377A24C37}" name="Energie (kWh) CPU avec kube-downscaler" totalsRowFunction="sum" dataDxfId="8">
       <calculatedColumnFormula array="1">Tableau1[[#This Row],[CPUmoy (Période active)]]*Tableau1[[#This Row],[Nb heures (période active) par an]]*Tableau2[kWh/CPU]*Tableau2[PUE]*Tableau1[[#This Row],[Nb de pods]]</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="13" xr3:uid="{A03F9329-AF52-4DA6-BCDF-578A92D93474}" name="Energie (kWh) RAM avec kube-downscaler" totalsRowFunction="sum" dataDxfId="2">
+    <tableColumn id="13" xr3:uid="{A03F9329-AF52-4DA6-BCDF-578A92D93474}" name="Energie (kWh) RAM avec kube-downscaler" totalsRowFunction="sum" dataDxfId="7">
       <calculatedColumnFormula array="1">Tableau1[[#This Row],[RAMmoy (Période active)]]*Tableau1[[#This Row],[Nb heures (période active) par an]]*Tableau2[kWh/GoRAM]*Tableau2[PUE]*Tableau1[[#This Row],[Nb de pods]]</calculatedColumnFormula>
     </tableColumn>
     <tableColumn id="15" xr3:uid="{5D8FBA35-CDBA-4C68-9E83-6835799B882B}" name="Energie (kWh) totale avec kube-downscaler" totalsRowFunction="sum">
@@ -723,9 +719,9 @@
     <tableColumn id="17" xr3:uid="{73C1DC75-42DF-478E-8AD5-15C822BC4D8D}" name="kgCO2eq avec kube-downscaler" totalsRowFunction="sum">
       <calculatedColumnFormula array="1">Tableau1[[#This Row],[Energie (kWh) totale avec kube-downscaler]]*Tableau2[kgCO2/kWh]</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="20" xr3:uid="{682833CB-1513-4B10-9167-85793868C041}" name="Gain" totalsRowFunction="custom" dataDxfId="1" totalsRowDxfId="0" dataCellStyle="Pourcentage">
-      <calculatedColumnFormula>Tableau1[[#This Row],[kgCO2eq avec kube-downscaler]]/Tableau1[[#This Row],[kgCO2eq sans kube-downscaler]]</calculatedColumnFormula>
-      <totalsRowFormula>Tableau1[[#Totals],[kgCO2eq avec kube-downscaler]]/Tableau1[[#Totals],[kgCO2eq sans kube-downscaler]]</totalsRowFormula>
+    <tableColumn id="20" xr3:uid="{682833CB-1513-4B10-9167-85793868C041}" name="Evolution" totalsRowFunction="custom" dataDxfId="1" totalsRowDxfId="0" dataCellStyle="Pourcentage">
+      <calculatedColumnFormula>(Tableau1[[#This Row],[kgCO2eq avec kube-downscaler]]-Tableau1[[#This Row],[kgCO2eq sans kube-downscaler]])/Tableau1[[#This Row],[kgCO2eq sans kube-downscaler]]</calculatedColumnFormula>
+      <totalsRowFormula>(Tableau1[[#Totals],[kgCO2eq avec kube-downscaler]]-Tableau1[[#Totals],[kgCO2eq sans kube-downscaler]])/Tableau1[[#Totals],[kgCO2eq sans kube-downscaler]]</totalsRowFormula>
     </tableColumn>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium4" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
@@ -733,10 +729,10 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{B2C602C2-FA01-4AEB-A7CE-4FFF16AEA4C4}" name="Tableau2" displayName="Tableau2" ref="A1:D2" totalsRowShown="0" headerRowDxfId="10" headerRowBorderDxfId="9" tableBorderDxfId="8" totalsRowBorderDxfId="7">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{B2C602C2-FA01-4AEB-A7CE-4FFF16AEA4C4}" name="Tableau2" displayName="Tableau2" ref="A1:D2" totalsRowShown="0" headerRowDxfId="6" headerRowBorderDxfId="5" tableBorderDxfId="4" totalsRowBorderDxfId="3">
   <autoFilter ref="A1:D2" xr:uid="{B2C602C2-FA01-4AEB-A7CE-4FFF16AEA4C4}"/>
   <tableColumns count="4">
-    <tableColumn id="1" xr3:uid="{75E3BE52-84B4-4CA9-A8BC-59D3569696C3}" name="kWh/CPU" dataDxfId="6">
+    <tableColumn id="1" xr3:uid="{75E3BE52-84B4-4CA9-A8BC-59D3569696C3}" name="kWh/CPU" dataDxfId="2">
       <calculatedColumnFormula>2.12/1000</calculatedColumnFormula>
     </tableColumn>
     <tableColumn id="2" xr3:uid="{68416F37-1DE6-4D24-8166-24F56C99900B}" name="kWh/GoRAM">
@@ -1070,8 +1066,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{97F58A1D-C50B-4ECA-A024-B8F8F3E1F1E5}">
   <dimension ref="A1:R9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F4" sqref="F4"/>
+    <sheetView tabSelected="1" zoomScale="93" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="Q12" sqref="Q12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" outlineLevelCol="1" x14ac:dyDescent="0.3"/>
@@ -1097,84 +1093,84 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A1" s="11" t="s">
+      <c r="A1" s="21" t="s">
+        <v>28</v>
+      </c>
+      <c r="B1" s="21"/>
+      <c r="C1" s="21"/>
+      <c r="D1" s="21"/>
+      <c r="E1" s="21"/>
+      <c r="F1" s="21"/>
+      <c r="G1" s="21"/>
+      <c r="H1" s="21"/>
+      <c r="I1" s="21"/>
+      <c r="J1" s="22" t="s">
         <v>29</v>
       </c>
-      <c r="B1" s="11"/>
-      <c r="C1" s="11"/>
-      <c r="D1" s="11"/>
-      <c r="E1" s="11"/>
-      <c r="F1" s="11"/>
-      <c r="G1" s="11"/>
-      <c r="H1" s="11"/>
-      <c r="I1" s="11"/>
-      <c r="J1" s="12" t="s">
+      <c r="K1" s="22"/>
+      <c r="L1" s="22"/>
+      <c r="M1" s="22"/>
+      <c r="N1" s="22"/>
+      <c r="O1" s="22"/>
+      <c r="P1" s="22"/>
+      <c r="Q1" s="22"/>
+    </row>
+    <row r="2" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A2" s="23" t="s">
         <v>30</v>
       </c>
-      <c r="K1" s="12"/>
-      <c r="L1" s="12"/>
-      <c r="M1" s="12"/>
-      <c r="N1" s="12"/>
-      <c r="O1" s="12"/>
-      <c r="P1" s="12"/>
-      <c r="Q1" s="12"/>
-    </row>
-    <row r="2" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A2" s="13" t="s">
-        <v>31</v>
-      </c>
-      <c r="B2" s="13"/>
-      <c r="C2" s="13"/>
-      <c r="D2" s="14" t="s">
+      <c r="B2" s="23"/>
+      <c r="C2" s="23"/>
+      <c r="D2" s="24" t="s">
+        <v>13</v>
+      </c>
+      <c r="E2" s="24"/>
+      <c r="F2" s="25" t="s">
         <v>14</v>
       </c>
-      <c r="E2" s="14"/>
-      <c r="F2" s="15" t="s">
+      <c r="G2" s="25"/>
+      <c r="H2" s="26" t="s">
         <v>15</v>
       </c>
-      <c r="G2" s="15"/>
-      <c r="H2" s="16" t="s">
+      <c r="I2" s="26"/>
+      <c r="J2" s="27" t="s">
         <v>16</v>
       </c>
-      <c r="I2" s="16"/>
-      <c r="J2" s="17" t="s">
+      <c r="K2" s="27"/>
+      <c r="L2" s="27"/>
+      <c r="M2" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="N2" s="20" t="s">
         <v>17</v>
       </c>
-      <c r="K2" s="17"/>
-      <c r="L2" s="17"/>
-      <c r="M2" s="3" t="s">
+      <c r="O2" s="20"/>
+      <c r="P2" s="20"/>
+      <c r="Q2" s="4" t="s">
         <v>19</v>
-      </c>
-      <c r="N2" s="10" t="s">
-        <v>18</v>
-      </c>
-      <c r="O2" s="10"/>
-      <c r="P2" s="10"/>
-      <c r="Q2" s="4" t="s">
-        <v>20</v>
       </c>
     </row>
     <row r="3" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
+        <v>21</v>
+      </c>
+      <c r="B3" t="s">
         <v>22</v>
       </c>
-      <c r="B3" t="s">
+      <c r="C3" t="s">
         <v>23</v>
       </c>
-      <c r="C3" t="s">
+      <c r="D3" t="s">
         <v>24</v>
       </c>
-      <c r="D3" t="s">
+      <c r="E3" t="s">
         <v>25</v>
       </c>
-      <c r="E3" t="s">
+      <c r="F3" t="s">
         <v>26</v>
       </c>
-      <c r="F3" t="s">
+      <c r="G3" t="s">
         <v>27</v>
-      </c>
-      <c r="G3" t="s">
-        <v>28</v>
       </c>
       <c r="H3" t="s">
         <v>11</v>
@@ -1207,15 +1203,15 @@
         <v>10</v>
       </c>
       <c r="R3" t="s">
-        <v>13</v>
+        <v>77</v>
       </c>
     </row>
     <row r="4" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B4" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C4">
         <v>2</v>
@@ -1273,16 +1269,16 @@
         <v>0.86381568000000009</v>
       </c>
       <c r="R4" s="2">
-        <f>Tableau1[[#This Row],[kgCO2eq avec kube-downscaler]]/Tableau1[[#This Row],[kgCO2eq sans kube-downscaler]]</f>
-        <v>0.47391939123125248</v>
+        <f>(Tableau1[[#This Row],[kgCO2eq avec kube-downscaler]]-Tableau1[[#This Row],[kgCO2eq sans kube-downscaler]])/Tableau1[[#This Row],[kgCO2eq sans kube-downscaler]]</f>
+        <v>-0.52608060876874752</v>
       </c>
     </row>
     <row r="5" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B5" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C5">
         <v>2</v>
@@ -1307,11 +1303,11 @@
         <f>24*365-Tableau1[[#This Row],[Nb heures (période active) par an]]</f>
         <v>5640</v>
       </c>
-      <c r="J5" s="18" cm="1">
+      <c r="J5" cm="1">
         <f t="array" ref="J5">(Tableau1[[#This Row],[CPUmoy (Période active)]]*Tableau1[[#This Row],[Nb heures (période active) par an]]+Tableau1[[#This Row],[CPUmoy (période inactive)]]*Tableau1[[#This Row],[Nb heures (période inactive) par an]])*Tableau2[kWh/CPU]*Tableau2[PUE]*Tableau1[[#This Row],[Nb de pods]]</f>
         <v>17.095679999999998</v>
       </c>
-      <c r="K5" s="18" cm="1">
+      <c r="K5" cm="1">
         <f t="array" ref="K5">(Tableau1[[#This Row],[RAMmoy (Période active)]]*Tableau1[[#This Row],[Nb heures (période active) par an]]+Tableau1[[#This Row],[RAMmoy (période inactive)]]*Tableau1[[#This Row],[Nb heures (période inactive) par an]])*Tableau2[kWh/GoRAM]*Tableau2[PUE]*Tableau1[[#This Row],[Nb de pods]]</f>
         <v>15.452640000000002</v>
       </c>
@@ -1323,11 +1319,11 @@
         <f t="array" ref="M5">Tableau1[[#This Row],[Energie (kWh) totale sans kube-downscaler]]*Tableau2[kgCO2/kWh]</f>
         <v>1.8227059200000002</v>
       </c>
-      <c r="N5" s="18" cm="1">
+      <c r="N5" cm="1">
         <f t="array" ref="N5">Tableau1[[#This Row],[CPUmoy (Période active)]]*Tableau1[[#This Row],[Nb heures (période active) par an]]*Tableau2[kWh/CPU]*Tableau2[PUE]*Tableau1[[#This Row],[Nb de pods]]</f>
         <v>9.9215999999999998</v>
       </c>
-      <c r="O5" s="18" cm="1">
+      <c r="O5" cm="1">
         <f t="array" ref="O5">Tableau1[[#This Row],[RAMmoy (Période active)]]*Tableau1[[#This Row],[Nb heures (période active) par an]]*Tableau2[kWh/GoRAM]*Tableau2[PUE]*Tableau1[[#This Row],[Nb de pods]]</f>
         <v>5.503680000000001</v>
       </c>
@@ -1340,16 +1336,16 @@
         <v>0.86381568000000009</v>
       </c>
       <c r="R5" s="2">
-        <f>Tableau1[[#This Row],[kgCO2eq avec kube-downscaler]]/Tableau1[[#This Row],[kgCO2eq sans kube-downscaler]]</f>
-        <v>0.47391939123125248</v>
+        <f>(Tableau1[[#This Row],[kgCO2eq avec kube-downscaler]]-Tableau1[[#This Row],[kgCO2eq sans kube-downscaler]])/Tableau1[[#This Row],[kgCO2eq sans kube-downscaler]]</f>
+        <v>-0.52608060876874752</v>
       </c>
     </row>
     <row r="6" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B6" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C6">
         <v>3</v>
@@ -1374,11 +1370,11 @@
         <f>24*365-Tableau1[[#This Row],[Nb heures (période active) par an]]</f>
         <v>5640</v>
       </c>
-      <c r="J6" s="18" cm="1">
+      <c r="J6" cm="1">
         <f t="array" ref="J6">(Tableau1[[#This Row],[CPUmoy (Période active)]]*Tableau1[[#This Row],[Nb heures (période active) par an]]+Tableau1[[#This Row],[CPUmoy (période inactive)]]*Tableau1[[#This Row],[Nb heures (période inactive) par an]])*Tableau2[kWh/CPU]*Tableau2[PUE]*Tableau1[[#This Row],[Nb de pods]]</f>
         <v>36.977039999999995</v>
       </c>
-      <c r="K6" s="18" cm="1">
+      <c r="K6" cm="1">
         <f t="array" ref="K6">(Tableau1[[#This Row],[RAMmoy (Période active)]]*Tableau1[[#This Row],[Nb heures (période active) par an]]+Tableau1[[#This Row],[RAMmoy (période inactive)]]*Tableau1[[#This Row],[Nb heures (période inactive) par an]])*Tableau2[kWh/GoRAM]*Tableau2[PUE]*Tableau1[[#This Row],[Nb de pods]]</f>
         <v>23.178960000000004</v>
       </c>
@@ -1390,11 +1386,11 @@
         <f t="array" ref="M6">Tableau1[[#This Row],[Energie (kWh) totale sans kube-downscaler]]*Tableau2[kgCO2/kWh]</f>
         <v>3.3687360000000002</v>
       </c>
-      <c r="N6" s="18" cm="1">
+      <c r="N6" cm="1">
         <f t="array" ref="N6">Tableau1[[#This Row],[CPUmoy (Période active)]]*Tableau1[[#This Row],[Nb heures (période active) par an]]*Tableau2[kWh/CPU]*Tableau2[PUE]*Tableau1[[#This Row],[Nb de pods]]</f>
         <v>20.835359999999998</v>
       </c>
-      <c r="O6" s="18" cm="1">
+      <c r="O6" cm="1">
         <f t="array" ref="O6">Tableau1[[#This Row],[RAMmoy (Période active)]]*Tableau1[[#This Row],[Nb heures (période active) par an]]*Tableau2[kWh/GoRAM]*Tableau2[PUE]*Tableau1[[#This Row],[Nb de pods]]</f>
         <v>8.2555200000000006</v>
       </c>
@@ -1407,16 +1403,16 @@
         <v>1.6290892799999999</v>
       </c>
       <c r="R6" s="2">
-        <f>Tableau1[[#This Row],[kgCO2eq avec kube-downscaler]]/Tableau1[[#This Row],[kgCO2eq sans kube-downscaler]]</f>
-        <v>0.48359066427289044</v>
+        <f>(Tableau1[[#This Row],[kgCO2eq avec kube-downscaler]]-Tableau1[[#This Row],[kgCO2eq sans kube-downscaler]])/Tableau1[[#This Row],[kgCO2eq sans kube-downscaler]]</f>
+        <v>-0.51640933572710956</v>
       </c>
     </row>
     <row r="7" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B7" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C7">
         <v>5</v>
@@ -1441,11 +1437,11 @@
         <f>24*365-Tableau1[[#This Row],[Nb heures (période active) par an]]</f>
         <v>5640</v>
       </c>
-      <c r="J7" s="18" cm="1">
+      <c r="J7" cm="1">
         <f t="array" ref="J7">(Tableau1[[#This Row],[CPUmoy (Période active)]]*Tableau1[[#This Row],[Nb heures (période active) par an]]+Tableau1[[#This Row],[CPUmoy (période inactive)]]*Tableau1[[#This Row],[Nb heures (période inactive) par an]])*Tableau2[kWh/CPU]*Tableau2[PUE]*Tableau1[[#This Row],[Nb de pods]]</f>
         <v>76.510800000000003</v>
       </c>
-      <c r="K7" s="18" cm="1">
+      <c r="K7" cm="1">
         <f t="array" ref="K7">(Tableau1[[#This Row],[RAMmoy (Période active)]]*Tableau1[[#This Row],[Nb heures (période active) par an]]+Tableau1[[#This Row],[RAMmoy (période inactive)]]*Tableau1[[#This Row],[Nb heures (période inactive) par an]])*Tableau2[kWh/GoRAM]*Tableau2[PUE]*Tableau1[[#This Row],[Nb de pods]]</f>
         <v>46.357920000000007</v>
       </c>
@@ -1457,11 +1453,11 @@
         <f t="array" ref="M7">Tableau1[[#This Row],[Energie (kWh) totale sans kube-downscaler]]*Tableau2[kgCO2/kWh]</f>
         <v>6.8806483200000006</v>
       </c>
-      <c r="N7" s="18" cm="1">
+      <c r="N7" cm="1">
         <f t="array" ref="N7">Tableau1[[#This Row],[CPUmoy (Période active)]]*Tableau1[[#This Row],[Nb heures (période active) par an]]*Tableau2[kWh/CPU]*Tableau2[PUE]*Tableau1[[#This Row],[Nb de pods]]</f>
         <v>49.607999999999997</v>
       </c>
-      <c r="O7" s="18" cm="1">
+      <c r="O7" cm="1">
         <f t="array" ref="O7">Tableau1[[#This Row],[RAMmoy (Période active)]]*Tableau1[[#This Row],[Nb heures (période active) par an]]*Tableau2[kWh/GoRAM]*Tableau2[PUE]*Tableau1[[#This Row],[Nb de pods]]</f>
         <v>16.511040000000001</v>
       </c>
@@ -1474,16 +1470,16 @@
         <v>3.7026662400000001</v>
       </c>
       <c r="R7" s="2">
-        <f>Tableau1[[#This Row],[kgCO2eq avec kube-downscaler]]/Tableau1[[#This Row],[kgCO2eq sans kube-downscaler]]</f>
-        <v>0.53812752342500192</v>
+        <f>(Tableau1[[#This Row],[kgCO2eq avec kube-downscaler]]-Tableau1[[#This Row],[kgCO2eq sans kube-downscaler]])/Tableau1[[#This Row],[kgCO2eq sans kube-downscaler]]</f>
+        <v>-0.46187247657499814</v>
       </c>
     </row>
     <row r="8" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B8" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C8">
         <v>5</v>
@@ -1508,11 +1504,11 @@
         <f>24*365-Tableau1[[#This Row],[Nb heures (période active) par an]]</f>
         <v>5640</v>
       </c>
-      <c r="J8" s="18" cm="1">
+      <c r="J8" cm="1">
         <f t="array" ref="J8">(Tableau1[[#This Row],[CPUmoy (Période active)]]*Tableau1[[#This Row],[Nb heures (période active) par an]]+Tableau1[[#This Row],[CPUmoy (période inactive)]]*Tableau1[[#This Row],[Nb heures (période inactive) par an]])*Tableau2[kWh/CPU]*Tableau2[PUE]*Tableau1[[#This Row],[Nb de pods]]</f>
         <v>76.510800000000003</v>
       </c>
-      <c r="K8" s="18" cm="1">
+      <c r="K8" cm="1">
         <f t="array" ref="K8">(Tableau1[[#This Row],[RAMmoy (Période active)]]*Tableau1[[#This Row],[Nb heures (période active) par an]]+Tableau1[[#This Row],[RAMmoy (période inactive)]]*Tableau1[[#This Row],[Nb heures (période inactive) par an]])*Tableau2[kWh/GoRAM]*Tableau2[PUE]*Tableau1[[#This Row],[Nb de pods]]</f>
         <v>46.357920000000007</v>
       </c>
@@ -1524,11 +1520,11 @@
         <f t="array" ref="M8">Tableau1[[#This Row],[Energie (kWh) totale sans kube-downscaler]]*Tableau2[kgCO2/kWh]</f>
         <v>6.8806483200000006</v>
       </c>
-      <c r="N8" s="18" cm="1">
+      <c r="N8" cm="1">
         <f t="array" ref="N8">Tableau1[[#This Row],[CPUmoy (Période active)]]*Tableau1[[#This Row],[Nb heures (période active) par an]]*Tableau2[kWh/CPU]*Tableau2[PUE]*Tableau1[[#This Row],[Nb de pods]]</f>
         <v>49.607999999999997</v>
       </c>
-      <c r="O8" s="18" cm="1">
+      <c r="O8" cm="1">
         <f t="array" ref="O8">Tableau1[[#This Row],[RAMmoy (Période active)]]*Tableau1[[#This Row],[Nb heures (période active) par an]]*Tableau2[kWh/GoRAM]*Tableau2[PUE]*Tableau1[[#This Row],[Nb de pods]]</f>
         <v>16.511040000000001</v>
       </c>
@@ -1541,13 +1537,13 @@
         <v>3.7026662400000001</v>
       </c>
       <c r="R8" s="2">
-        <f>Tableau1[[#This Row],[kgCO2eq avec kube-downscaler]]/Tableau1[[#This Row],[kgCO2eq sans kube-downscaler]]</f>
-        <v>0.53812752342500192</v>
+        <f>(Tableau1[[#This Row],[kgCO2eq avec kube-downscaler]]-Tableau1[[#This Row],[kgCO2eq sans kube-downscaler]])/Tableau1[[#This Row],[kgCO2eq sans kube-downscaler]]</f>
+        <v>-0.46187247657499814</v>
       </c>
     </row>
     <row r="9" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="J9">
         <f>SUBTOTAL(109,Tableau1[Energie (kWh) CPU sans kube-downscaler])</f>
@@ -1581,9 +1577,9 @@
         <f>SUBTOTAL(109,Tableau1[kgCO2eq avec kube-downscaler])</f>
         <v>10.762053120000001</v>
       </c>
-      <c r="R9" s="19">
-        <f>Tableau1[[#Totals],[kgCO2eq avec kube-downscaler]]/Tableau1[[#Totals],[kgCO2eq sans kube-downscaler]]</f>
-        <v>0.51801794808098367</v>
+      <c r="R9" s="10">
+        <f>(Tableau1[[#Totals],[kgCO2eq avec kube-downscaler]]-Tableau1[[#Totals],[kgCO2eq sans kube-downscaler]])/Tableau1[[#Totals],[kgCO2eq sans kube-downscaler]]</f>
+        <v>-0.48198205191901633</v>
       </c>
     </row>
   </sheetData>
@@ -1629,7 +1625,7 @@
         <v>2</v>
       </c>
       <c r="D1" s="5" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.3">
@@ -1682,208 +1678,208 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A1" s="30" t="s">
+      <c r="A1" s="28" t="s">
+        <v>38</v>
+      </c>
+      <c r="B1" s="28"/>
+      <c r="C1" s="28"/>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A2" s="13" t="s">
+        <v>40</v>
+      </c>
+      <c r="B2" s="13" t="s">
+        <v>41</v>
+      </c>
+      <c r="C2" s="13" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A3" s="14" t="s">
         <v>39</v>
       </c>
-      <c r="B1" s="30"/>
-      <c r="C1" s="30"/>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A2" s="22" t="s">
-        <v>41</v>
-      </c>
-      <c r="B2" s="22" t="s">
+      <c r="B3" s="15" t="s">
         <v>42</v>
       </c>
-      <c r="C2" s="22" t="s">
+      <c r="C3" s="16" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="3" spans="1:3" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A3" s="23" t="s">
-        <v>40</v>
-      </c>
-      <c r="B3" s="24" t="s">
-        <v>43</v>
-      </c>
-      <c r="C3" s="25" t="s">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A4" s="14" t="s">
         <v>45</v>
       </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A4" s="23" t="s">
+      <c r="B4" s="15" t="s">
+        <v>42</v>
+      </c>
+      <c r="C4" s="14"/>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A5" s="14" t="s">
+        <v>76</v>
+      </c>
+      <c r="B5" s="15" t="s">
         <v>46</v>
       </c>
-      <c r="B4" s="24" t="s">
-        <v>43</v>
-      </c>
-      <c r="C4" s="23"/>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A5" s="23" t="s">
-        <v>77</v>
-      </c>
-      <c r="B5" s="24" t="s">
+      <c r="C5" s="14" t="s">
         <v>47</v>
       </c>
-      <c r="C5" s="23" t="s">
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A6" s="14" t="s">
         <v>48</v>
       </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A6" s="23" t="s">
+      <c r="B6" s="14"/>
+      <c r="C6" s="14" t="s">
         <v>49</v>
       </c>
-      <c r="B6" s="23"/>
-      <c r="C6" s="23" t="s">
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A8" s="29" t="s">
+        <v>53</v>
+      </c>
+      <c r="B8" s="29"/>
+      <c r="C8" s="29"/>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A9" s="18" t="s">
+        <v>54</v>
+      </c>
+      <c r="B9" s="19" t="s">
+        <v>55</v>
+      </c>
+      <c r="C9" s="19" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A10" s="16" t="s">
+        <v>21</v>
+      </c>
+      <c r="B10" s="12" t="s">
+        <v>57</v>
+      </c>
+      <c r="C10" s="12" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A11" s="16" t="s">
+        <v>22</v>
+      </c>
+      <c r="B11" s="12" t="s">
+        <v>59</v>
+      </c>
+      <c r="C11" s="12" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A12" s="16" t="s">
+        <v>23</v>
+      </c>
+      <c r="B12" s="12" t="s">
+        <v>60</v>
+      </c>
+      <c r="C12" s="12" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A13" s="16" t="s">
+        <v>24</v>
+      </c>
+      <c r="B13" s="12" t="s">
+        <v>63</v>
+      </c>
+      <c r="C13" s="12" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A14" s="12" t="s">
+        <v>65</v>
+      </c>
+      <c r="B14" s="12" t="s">
+        <v>66</v>
+      </c>
+      <c r="C14" s="12" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A15" s="16" t="s">
+        <v>26</v>
+      </c>
+      <c r="B15" s="12" t="s">
+        <v>68</v>
+      </c>
+      <c r="C15" s="12" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A16" s="12" t="s">
+        <v>70</v>
+      </c>
+      <c r="B16" s="12" t="s">
+        <v>69</v>
+      </c>
+      <c r="C16" s="12" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A17" s="11"/>
+      <c r="B17" s="11"/>
+      <c r="C17" s="11"/>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A18" s="31" t="s">
         <v>50</v>
       </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A8" s="31" t="s">
-        <v>54</v>
-      </c>
-      <c r="B8" s="31"/>
-      <c r="C8" s="31"/>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A9" s="28" t="s">
-        <v>55</v>
-      </c>
-      <c r="B9" s="29" t="s">
-        <v>56</v>
-      </c>
-      <c r="C9" s="29" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A10" s="27" t="s">
-        <v>22</v>
-      </c>
-      <c r="B10" s="21" t="s">
-        <v>58</v>
-      </c>
-      <c r="C10" s="21" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A11" s="27" t="s">
-        <v>23</v>
-      </c>
-      <c r="B11" s="21" t="s">
-        <v>60</v>
-      </c>
-      <c r="C11" s="21" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A12" s="27" t="s">
-        <v>24</v>
-      </c>
-      <c r="B12" s="21" t="s">
-        <v>61</v>
-      </c>
-      <c r="C12" s="21" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A13" s="27" t="s">
-        <v>25</v>
-      </c>
-      <c r="B13" s="21" t="s">
-        <v>64</v>
-      </c>
-      <c r="C13" s="21" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A14" s="21" t="s">
-        <v>66</v>
-      </c>
-      <c r="B14" s="21" t="s">
-        <v>67</v>
-      </c>
-      <c r="C14" s="21" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A15" s="27" t="s">
-        <v>27</v>
-      </c>
-      <c r="B15" s="21" t="s">
-        <v>69</v>
-      </c>
-      <c r="C15" s="21" t="s">
+      <c r="B18" s="32"/>
+      <c r="C18" s="32"/>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A19" s="30" t="s">
+        <v>51</v>
+      </c>
+      <c r="B19" s="30"/>
+      <c r="C19" s="30"/>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A20" s="30" t="s">
+        <v>52</v>
+      </c>
+      <c r="B20" s="30"/>
+      <c r="C20" s="30"/>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A21" s="33" t="s">
         <v>73</v>
       </c>
-    </row>
-    <row r="16" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A16" s="21" t="s">
-        <v>71</v>
-      </c>
-      <c r="B16" s="21" t="s">
-        <v>70</v>
-      </c>
-      <c r="C16" s="21" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A17" s="20"/>
-      <c r="B17" s="20"/>
-      <c r="C17" s="20"/>
-    </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A18" s="32" t="s">
-        <v>51</v>
-      </c>
-      <c r="B18" s="33"/>
-      <c r="C18" s="33"/>
-    </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A19" s="34" t="s">
-        <v>52</v>
-      </c>
-      <c r="B19" s="34"/>
-      <c r="C19" s="34"/>
-    </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A20" s="34" t="s">
-        <v>53</v>
-      </c>
-      <c r="B20" s="34"/>
-      <c r="C20" s="34"/>
-    </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A21" s="35" t="s">
+      <c r="B21" s="33"/>
+      <c r="C21" s="33"/>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A22" s="33" t="s">
         <v>74</v>
       </c>
-      <c r="B21" s="35"/>
-      <c r="C21" s="35"/>
-    </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A22" s="35" t="s">
+      <c r="B22" s="33"/>
+      <c r="C22" s="33"/>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A23" s="30" t="s">
         <v>75</v>
       </c>
-      <c r="B22" s="35"/>
-      <c r="C22" s="35"/>
-    </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A23" s="34" t="s">
-        <v>76</v>
-      </c>
-      <c r="B23" s="34"/>
-      <c r="C23" s="34"/>
+      <c r="B23" s="30"/>
+      <c r="C23" s="30"/>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="B24" s="26"/>
-      <c r="C24" s="26"/>
+      <c r="B24" s="17"/>
+      <c r="C24" s="17"/>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A26" s="9"/>

</xml_diff>